<commit_message>
Plot updated spatiotemporal model
Change simulated datasets to reflect changes in the spatiotemporal model estimates
</commit_message>
<xml_diff>
--- a/analysis/models/MATLAB/experiment_2/collated_exp2.xlsx
+++ b/analysis/models/MATLAB/experiment_2/collated_exp2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Documents\git\sourcemem_online\analysis\models\MATLAB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Documents\git\sourcemem_online\analysis\models\MATLAB\experiment_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81B89D3D-F367-45C4-93EE-3229B7DE71D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BAD95B-764E-4EF1-B6D1-FBF1E9F1D052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{43BA5041-B1E9-49D4-972E-6E10B4A41A7D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="2" xr2:uid="{43BA5041-B1E9-49D4-972E-6E10B4A41A7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Flat Intrusion" sheetId="4" r:id="rId1"/>
@@ -780,7 +780,7 @@
         <v>4.1694599999999999</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:T7" si="0">AVERAGE(E2:E6)</f>
+        <f t="shared" ref="E7:O7" si="0">AVERAGE(E2:E6)</f>
         <v>0</v>
       </c>
       <c r="F7">
@@ -1185,7 +1185,7 @@
         <v>3.7314480000000003</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:T7" si="0">AVERAGE(E2:E6)</f>
+        <f t="shared" ref="E7:R7" si="0">AVERAGE(E2:E6)</f>
         <v>0</v>
       </c>
       <c r="F7">
@@ -1250,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9852AA22-EE05-4C6B-BD5D-97574FDF58E6}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1574,55 +1574,55 @@
         <v>21</v>
       </c>
       <c r="C6">
-        <v>4052.0762</v>
+        <v>4039.4268033950002</v>
       </c>
       <c r="D6">
-        <v>0.39643</v>
+        <v>4.6098403848728902</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>2.2029999999999998</v>
+        <v>0.288468766059159</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0.90151999999999999</v>
+        <v>0.53383034567051602</v>
       </c>
       <c r="I6">
-        <v>2.4884E-2</v>
+        <v>0.27702017411214502</v>
       </c>
       <c r="J6">
-        <v>0.86107999999999996</v>
+        <v>1.7845357201518699</v>
       </c>
       <c r="K6">
-        <v>1.841</v>
+        <v>0.66460491603462701</v>
       </c>
       <c r="L6">
-        <v>0.15789</v>
+        <v>0.18605278237171399</v>
       </c>
       <c r="M6">
-        <v>0.13394</v>
+        <v>0.74313567631079402</v>
       </c>
       <c r="N6">
-        <v>0.90124000000000004</v>
+        <v>0.49834392802584299</v>
       </c>
       <c r="O6">
-        <v>0.68201999999999996</v>
+        <v>0.448185970392319</v>
       </c>
       <c r="P6">
-        <v>0.61414999999999997</v>
+        <v>0.89270664352491302</v>
       </c>
       <c r="Q6">
-        <v>0.49179</v>
+        <v>0.66353831843727196</v>
       </c>
       <c r="R6">
-        <v>0.85568</v>
+        <v>0.83172412895627701</v>
       </c>
       <c r="S6">
-        <v>0.23011000000000001</v>
+        <v>0.26400088840503799</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -1631,74 +1631,74 @@
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C7">
         <f>SUM(C2:C6)</f>
-        <v>16297.35</v>
+        <v>16284.700603395002</v>
       </c>
       <c r="D7">
         <f>AVERAGE(D2:D6)</f>
-        <v>3.8354660000000003</v>
+        <v>4.678148076974578</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:V7" si="0">AVERAGE(E2:E6)</f>
+        <f>AVERAGE(E2:E6)</f>
         <v>0</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
-        <v>2.5751200000000001</v>
+        <f>AVERAGE(F2:F6)</f>
+        <v>2.1922137532118322</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(G2:G6)</f>
         <v>0</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
-        <v>0.46232200000000001</v>
+        <f>AVERAGE(H2:H6)</f>
+        <v>0.38878406913410318</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
-        <v>0.19235952000000001</v>
+        <f>AVERAGE(I2:I6)</f>
+        <v>0.24278675482242901</v>
       </c>
       <c r="J7">
-        <f t="shared" si="0"/>
-        <v>2.8536759999999997</v>
+        <f>AVERAGE(J2:J6)</f>
+        <v>3.0383671440303739</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
-        <v>1.6629999999999998</v>
+        <f>AVERAGE(K2:K6)</f>
+        <v>1.4277209832069253</v>
       </c>
       <c r="L7">
-        <f t="shared" si="0"/>
-        <v>9.653719999999999E-2</v>
+        <f>AVERAGE(L2:L6)</f>
+        <v>0.10216975647434279</v>
       </c>
       <c r="M7">
-        <f t="shared" si="0"/>
-        <v>0.15482319999999999</v>
+        <f>AVERAGE(M2:M6)</f>
+        <v>0.27666233526215878</v>
       </c>
       <c r="N7">
-        <f t="shared" si="0"/>
-        <v>0.64782600000000001</v>
+        <f>AVERAGE(N2:N6)</f>
+        <v>0.56724678560516861</v>
       </c>
       <c r="O7">
-        <f t="shared" si="0"/>
-        <v>0.46584999999999999</v>
+        <f>AVERAGE(O2:O6)</f>
+        <v>0.41908319407846378</v>
       </c>
       <c r="P7">
-        <f t="shared" si="0"/>
-        <v>0.71700000000000008</v>
+        <f>AVERAGE(P2:P6)</f>
+        <v>0.77271132870498271</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="0"/>
-        <v>0.72200600000000004</v>
+        <f>AVERAGE(Q2:Q6)</f>
+        <v>0.75635566368745444</v>
       </c>
       <c r="R7">
-        <f t="shared" si="0"/>
-        <v>0.71396599999999999</v>
+        <f>AVERAGE(R2:R6)</f>
+        <v>0.70917482579125546</v>
       </c>
       <c r="S7">
-        <f t="shared" si="0"/>
-        <v>6.8241893979999996E-2</v>
+        <f>AVERAGE(S2:S6)</f>
+        <v>7.502007166100759E-2</v>
       </c>
       <c r="T7">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(T2:T6)</f>
         <v>0</v>
       </c>
     </row>
@@ -2217,7 +2217,7 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:V7"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>